<commit_message>
tick MPIMP templates up one version to trigger swobup
</commit_message>
<xml_diff>
--- a/templates/community/MPIMP/MPIMP_Fernie_Chromatography.xlsx
+++ b/templates/community/MPIMP/MPIMP_Fernie_Chromatography.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\mpimp-golm\USER\HOMES\Wijesingha1055\GitHub\Swate-templates\templates\community\MPIMP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/community/MPIMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7CA3B7-E83E-4244-BD40-CC531B156859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="13512" activeTab="1"/>
+    <workbookView xWindow="-21340" yWindow="-21100" windowWidth="32740" windowHeight="20020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chromatography" sheetId="3" r:id="rId1"/>
@@ -20,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={84DDE716-575F-488F-A013-73DB8674E0F1}</author>
     <author>tc={8F078296-ACA9-4BE1-895A-22EBE1434F09}</author>
@@ -49,7 +39,7 @@
     <author>tc={D190F77A-D580-4D55-9D5B-23B8ED7B7DEC}</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -68,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="1" shapeId="0">
+    <comment ref="A2" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -85,7 +75,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="2" shapeId="0">
+    <comment ref="A3" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -102,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="3" shapeId="0">
+    <comment ref="A4" authorId="3" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -119,7 +109,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A5" authorId="4" shapeId="0">
+    <comment ref="A5" authorId="4" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -136,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A6" authorId="5" shapeId="0">
+    <comment ref="A6" authorId="5" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -153,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="6" shapeId="0">
+    <comment ref="A7" authorId="6" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
       <text>
         <r>
           <rPr>
@@ -170,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A11" authorId="7" shapeId="0">
+    <comment ref="A11" authorId="7" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
       <text>
         <r>
           <rPr>
@@ -187,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A15" authorId="8" shapeId="0">
+    <comment ref="A15" authorId="8" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
       <text>
         <r>
           <rPr>
@@ -448,9 +438,6 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -554,12 +541,15 @@
   </si>
   <si>
     <t>annotationTableBrightChipmunk5</t>
+  </si>
+  <si>
+    <t>1.0.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00\ &quot;microliter&quot;"/>
   </numFmts>
@@ -843,40 +833,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="annotationTableBrightChipmunk5" displayName="annotationTableBrightChipmunk5" ref="A1:AE5" totalsRowShown="0">
-  <autoFilter ref="A1:AE5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="annotationTableBrightChipmunk5" displayName="annotationTableBrightChipmunk5" ref="A1:AE5" totalsRowShown="0">
+  <autoFilter ref="A1:AE5" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="31">
-    <tableColumn id="1" name="Source Name"/>
-    <tableColumn id="25" name="Protocol Type" dataDxfId="28"/>
-    <tableColumn id="26" name="Term Source REF (DPBO:1000161)" dataDxfId="27"/>
-    <tableColumn id="27" name="Term Accession Number (DPBO:1000161)" dataDxfId="26"/>
-    <tableColumn id="28" name="Protocol REF" dataDxfId="25"/>
-    <tableColumn id="3" name="Characteristic [sample type]" dataDxfId="24"/>
-    <tableColumn id="4" name="Term Source REF (DPBO:0000064)" dataDxfId="23"/>
-    <tableColumn id="5" name="Term Accession Number (DPBO:0000064)" dataDxfId="22"/>
-    <tableColumn id="29" name="Parameter [polarity]" dataDxfId="21"/>
-    <tableColumn id="30" name="Term Source REF (PATO:0002186)" dataDxfId="20"/>
-    <tableColumn id="31" name="Term Accession Number (PATO:0002186)" dataDxfId="19"/>
-    <tableColumn id="21" name="Parameter [chromatography]" dataDxfId="18"/>
-    <tableColumn id="22" name="Term Source REF (MS:1000054)" dataDxfId="17"/>
-    <tableColumn id="23" name="Term Accession Number (MS:1000054)" dataDxfId="16"/>
-    <tableColumn id="6" name="Parameter [MS sample post-extraction]" dataDxfId="15"/>
-    <tableColumn id="7" name="Term Source REF (DPBO:0000043)" dataDxfId="14"/>
-    <tableColumn id="8" name="Term Accession Number (DPBO:0000043)" dataDxfId="13"/>
-    <tableColumn id="9" name="Parameter [open split]" dataDxfId="12"/>
-    <tableColumn id="10" name="Term Source REF (MS:1000065)" dataDxfId="11"/>
-    <tableColumn id="11" name="Term Accession Number (MS:1000065)" dataDxfId="10"/>
-    <tableColumn id="12" name="Parameter [chromatography injection volume]" dataDxfId="9"/>
-    <tableColumn id="24" name="Unit" dataDxfId="8"/>
-    <tableColumn id="13" name="Term Source REF (DPBO:0010014)" dataDxfId="7"/>
-    <tableColumn id="14" name="Term Accession Number (DPBO:0010014)" dataDxfId="6"/>
-    <tableColumn id="15" name="Parameter [Batch]" dataDxfId="5"/>
-    <tableColumn id="16" name="Term Source REF (NCIT:C67073)" dataDxfId="4"/>
-    <tableColumn id="17" name="Term Accession Number (NCIT:C67073)" dataDxfId="3"/>
-    <tableColumn id="18" name="Parameter [Order]" dataDxfId="2"/>
-    <tableColumn id="19" name="Term Source REF (NCIT:C42680)" dataDxfId="1"/>
-    <tableColumn id="20" name="Term Accession Number (NCIT:C42680)" dataDxfId="0"/>
-    <tableColumn id="2" name="Sample Name"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Source Name"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="Protocol Type" dataDxfId="28"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="Term Source REF (DPBO:1000161)" dataDxfId="27"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="Term Accession Number (DPBO:1000161)" dataDxfId="26"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="Protocol REF" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Characteristic [sample type]" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Term Source REF (DPBO:0000064)" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Term Accession Number (DPBO:0000064)" dataDxfId="22"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="Parameter [polarity]" dataDxfId="21"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="Term Source REF (PATO:0002186)" dataDxfId="20"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="Term Accession Number (PATO:0002186)" dataDxfId="19"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Parameter [chromatography]" dataDxfId="18"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Term Source REF (MS:1000054)" dataDxfId="17"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="Term Accession Number (MS:1000054)" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Parameter [MS sample post-extraction]" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Term Source REF (DPBO:0000043)" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Term Accession Number (DPBO:0000043)" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Parameter [open split]" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Term Source REF (MS:1000065)" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Term Accession Number (MS:1000065)" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Parameter [chromatography injection volume]" dataDxfId="9"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Unit" dataDxfId="8"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Term Source REF (DPBO:0010014)" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Term Accession Number (DPBO:0010014)" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Parameter [Batch]" dataDxfId="5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Term Source REF (NCIT:C67073)" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Term Accession Number (NCIT:C67073)" dataDxfId="3"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Parameter [Order]" dataDxfId="2"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="Term Source REF (NCIT:C42680)" dataDxfId="1"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="Term Accession Number (NCIT:C42680)" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1229,55 +1219,55 @@
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
-      <we:containsCustomFunctions xmlns=""/>
+      <we:containsCustomFunctions/>
     </a:ext>
   </we:extLst>
 </we:webextension>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="40" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.88671875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="29.44140625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="38.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="29.5" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="22" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="34" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="41" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="41.109375" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="41.1640625" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="23.6640625" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="39.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="39" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="45.44140625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="45.5" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="24" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="39" hidden="1" customWidth="1"/>
     <col min="20" max="20" width="20.33203125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="46.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5546875" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="15.88671875" hidden="1" customWidth="1"/>
-    <col min="24" max="24" width="19.88671875" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="46.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="15.83203125" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="19.83203125" hidden="1" customWidth="1"/>
     <col min="25" max="25" width="20" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="0" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="15.6640625" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="0" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1372,7 +1362,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>31</v>
       </c>
@@ -1447,7 +1437,7 @@
       <c r="AC2" s="1"/>
       <c r="AD2" s="1"/>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
@@ -1522,7 +1512,7 @@
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1591,7 +1581,7 @@
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>31</v>
       </c>
@@ -1670,21 +1660,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="57.109375" customWidth="1"/>
-    <col min="3" max="4" width="39.109375" customWidth="1"/>
+    <col min="2" max="2" width="57.1640625" customWidth="1"/>
+    <col min="3" max="4" width="39.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>74</v>
       </c>
@@ -1692,7 +1682,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>76</v>
       </c>
@@ -1700,93 +1690,93 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="B4" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="8" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="B5" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="B5" s="8" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="B6" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="9"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="9"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B8" s="10"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="B9" s="8"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="B10" s="8"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="B11" s="9"/>
+    </row>
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="B11" s="9"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>90</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>94</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>32</v>
@@ -1795,93 +1785,93 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B15" s="9"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="B16" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="B16" s="10" t="s">
+    </row>
+    <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="B17" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="8" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="B18" s="8"/>
+    </row>
+    <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="8"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="B19" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B19" s="8" t="s">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="B20" s="8"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="8"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="B21" s="8"/>
+    </row>
+    <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="8"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="B22" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="B22" s="8" t="s">
+    </row>
+    <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="B23" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B23" s="8" t="s">
+    </row>
+    <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="B24" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B24" s="8" t="s">
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="8"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="B26" s="8"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="B26" s="8"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="6" t="s">
-        <v>113</v>
       </c>
       <c r="B27" s="11"/>
     </row>

</xml_diff>

<commit_message>
fix excel copy / paste error
</commit_message>
<xml_diff>
--- a/templates/community/MPIMP/MPIMP_Fernie_Chromatography.xlsx
+++ b/templates/community/MPIMP/MPIMP_Fernie_Chromatography.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/community/MPIMP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7CA3B7-E83E-4244-BD40-CC531B156859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB4D92C9-15E7-DB49-821D-EFA629B8A238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21340" yWindow="-21100" windowWidth="32740" windowHeight="20020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22480" yWindow="-21100" windowWidth="32740" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chromatography" sheetId="3" r:id="rId1"/>
@@ -199,7 +199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="113">
   <si>
     <t>Source Name</t>
   </si>
@@ -351,9 +351,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16432</t>
-  </si>
-  <si>
     <t>Pooled Sample</t>
   </si>
   <si>
@@ -379,9 +376,6 @@
   </si>
   <si>
     <t>2</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NCIT_C16433</t>
   </si>
   <si>
     <t>standard</t>
@@ -1229,16 +1223,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="40" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="33" customWidth="1"/>
+    <col min="4" max="4" width="40" customWidth="1"/>
     <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38.83203125" hidden="1" customWidth="1"/>
@@ -1445,19 +1439,19 @@
         <v>32</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>38</v>
@@ -1469,31 +1463,31 @@
         <v>40</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N3" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>44</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="S3" s="1" t="s">
         <v>39</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U3" s="2">
         <v>2</v>
@@ -1502,12 +1496,12 @@
       <c r="W3" s="1"/>
       <c r="X3" s="1"/>
       <c r="Y3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z3" s="1"/>
       <c r="AA3" s="1"/>
       <c r="AB3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC3" s="1"/>
       <c r="AD3" s="1"/>
@@ -1520,46 +1514,46 @@
         <v>32</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>39</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
@@ -1571,12 +1565,12 @@
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
       <c r="Y4" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="Z4" s="1"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="AC4" s="1"/>
       <c r="AD4" s="1"/>
@@ -1589,46 +1583,46 @@
         <v>32</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>39</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>32</v>
       </c>
       <c r="N5" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>44</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
@@ -1640,12 +1634,12 @@
       <c r="W5" s="1"/>
       <c r="X5" s="1"/>
       <c r="Y5" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="AC5" s="1"/>
       <c r="AD5" s="1"/>
@@ -1663,7 +1657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1676,107 +1670,107 @@
   <sheetData>
     <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B8" s="10"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B11" s="9"/>
     </row>
     <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>32</v>
@@ -1787,91 +1781,91 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B18" s="8"/>
     </row>
     <row r="19" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B20" s="8"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B21" s="8"/>
     </row>
     <row r="22" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B25" s="8"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B26" s="8"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B27" s="11"/>
     </row>

</xml_diff>